<commit_message>
updated to add ESC info
</commit_message>
<xml_diff>
--- a/BuyList.xlsx
+++ b/BuyList.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holme\Desktop\RoboWars-IIT-Mandi\Robowars 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holme\Desktop\RoboWars-IIT-Mandi\RoboWars2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928D669F-5549-40B3-93A6-FAEC8DC6E13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014DD05F-400C-44B5-A537-2A0C08043C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -73,6 +82,12 @@
   </si>
   <si>
     <t>https://robu.in/product-category/batteries/batteries-batteries/lithium-polymer-battery-packs/bonka-li-po-battery/6-cell-22-2v-25-2v-bonka-li-po-battery-lithium-polymer-battery-packs/</t>
+  </si>
+  <si>
+    <t>Spintend 100A escs</t>
+  </si>
+  <si>
+    <t>is vsec, would give really good performance, really good startup, HFI supoorted</t>
   </si>
 </sst>
 </file>
@@ -393,7 +408,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="132" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,6 +460,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>8000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated buy list for batteries and esc
</commit_message>
<xml_diff>
--- a/BuyList.xlsx
+++ b/BuyList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holme\Desktop\RoboWars-IIT-Mandi\RoboWars2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014DD05F-400C-44B5-A537-2A0C08043C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B175F61B-BB9D-4F03-AAA7-945721C25D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Item</t>
   </si>
@@ -88,16 +88,111 @@
   </si>
   <si>
     <t>is vsec, would give really good performance, really good startup, HFI supoorted</t>
+  </si>
+  <si>
+    <t>https://www.technobotix.in/products/tattu-g-tech-3500mah-150c-22-2v-6s-lipo-battery/1781252000009101158</t>
+  </si>
+  <si>
+    <t>https://www.quadkart.in/tattu-r-line-version-5-0-1050mah-6s-22-2v-150c-lipo-battery-xt60/</t>
+  </si>
+  <si>
+    <t>https://robokits.co.in/batteries-chargers/drone-batteries/genx-power-premium-lipo-battery/genxpower-22.2v-lipo-batteries/genx-22.2v-6s-1550mah-95c-190c-premium-lipo-lithium-polymer-battery</t>
+  </si>
+  <si>
+    <t>150c 1050mAh</t>
+  </si>
+  <si>
+    <t>95c 1550mAh</t>
+  </si>
+  <si>
+    <t>Genx 6S for Drive</t>
+  </si>
+  <si>
+    <t>https://robokits.co.in/genxpower-22.2v-lipo-batteries</t>
+  </si>
+  <si>
+    <t>should it be separate batteries for drive and weapon - if yes then calculation for each</t>
+  </si>
+  <si>
+    <t>has high C + low C options - weapon + drive we could do</t>
+  </si>
+  <si>
+    <t>much cheaper than others - but 95 C instead of 150C, still high C - though C rating always overshot</t>
+  </si>
+  <si>
+    <t>lower C - useful for drive</t>
+  </si>
+  <si>
+    <t>ChinaHobbyLine</t>
+  </si>
+  <si>
+    <t>https://chinahobbyline.com/</t>
+  </si>
+  <si>
+    <t>internet says that best FPV batteries for the price - though would have to import</t>
+  </si>
+  <si>
+    <t>Ovonic</t>
+  </si>
+  <si>
+    <t>ships to india but only less than 100Wh</t>
+  </si>
+  <si>
+    <t>https://www.ovonicshop.com/</t>
+  </si>
+  <si>
+    <t>https://www.moglix.com/brands/ovonic</t>
+  </si>
+  <si>
+    <t>https://indianrobostore.com/category/drone-batteries/lipo-battery</t>
+  </si>
+  <si>
+    <t>Indian Robo Store</t>
+  </si>
+  <si>
+    <t>donno how reliable is the store</t>
+  </si>
+  <si>
+    <t>https://probots.co.in/red-brick-200a-bldc-esc-electronic-speed-controller-2-7s-bec-5v-5a.html</t>
+  </si>
+  <si>
+    <t>store trustable or not?</t>
+  </si>
+  <si>
+    <t>https://www.roboverse.in/product-page/red-brick-200a</t>
+  </si>
+  <si>
+    <t>trustable or not, also pre-order</t>
+  </si>
+  <si>
+    <t>https://rcdrone.top/products/red-brick-speed-controller?variant=43812668113120</t>
+  </si>
+  <si>
+    <t>says that no post tax - but aroung 80 dollars</t>
+  </si>
+  <si>
+    <t>6249+1500+600</t>
+  </si>
+  <si>
+    <t>https://www.desertcart.in/search?query=red+brick+esc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,13 +215,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,16 +503,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="132" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="2" max="2" width="51.21875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
     <col min="5" max="5" width="128.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -436,80 +534,222 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>6249</v>
+      <c r="D2" t="s">
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>5499</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>5499</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
-        <v>8000</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D11">
+        <v>1200</v>
+      </c>
+      <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>9999</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{C782FA17-257D-4E2D-A03E-9B276B61C6E7}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{19F62360-E516-4E83-A7CA-8C4D22B37893}"/>
+    <hyperlink ref="C18" r:id="rId3" xr:uid="{9A07740D-62C3-4D86-9AA1-72C4DB53236C}"/>
+    <hyperlink ref="C19" r:id="rId4" xr:uid="{5B7BFAB5-18D8-4611-B08E-21619A94CAC0}"/>
+    <hyperlink ref="C20" r:id="rId5" xr:uid="{4659D747-BDA5-4CC4-AB9F-486D2A002B1D}"/>
+    <hyperlink ref="C21" r:id="rId6" xr:uid="{4B69CD8D-EF3F-4B0A-930A-95A073770C2B}"/>
+    <hyperlink ref="C22" r:id="rId7" xr:uid="{56E1CFF2-AFE4-471F-ABE5-C44B168475A3}"/>
+    <hyperlink ref="C23" r:id="rId8" xr:uid="{E6A90B1C-309D-4132-93FE-28BABCF262C5}"/>
+    <hyperlink ref="C24" r:id="rId9" xr:uid="{8D1C24D2-1BB2-441D-B3DC-F652141967DB}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{CB05FD3D-FBC3-49C3-971B-60FD30088F74}"/>
+    <hyperlink ref="C6" r:id="rId11" xr:uid="{4F778E17-C2C6-4351-93BC-06B4189B40C3}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{2835074F-D5AE-4DA9-8FF4-3FF3F78B56BA}"/>
+    <hyperlink ref="C9" r:id="rId13" xr:uid="{F0D34BB1-6168-4BF9-B9EB-3FD8276B937B}"/>
+    <hyperlink ref="C2" r:id="rId14" xr:uid="{7F739382-EF5A-418E-BEFA-6B9DF5137F75}"/>
+    <hyperlink ref="C10" r:id="rId15" xr:uid="{39F0B860-48E1-41B5-BA81-4400ADC3BBAF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>